<commit_message>
Exec summary + better CP performance
</commit_message>
<xml_diff>
--- a/BayesianNetworks/CSP_stats_TAN_EM.xlsx
+++ b/BayesianNetworks/CSP_stats_TAN_EM.xlsx
@@ -8,29 +8,38 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Angel\Documents\BayesianPDG\BayesianNetworks\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5017A35D-662E-449D-9A86-B4FD9F85C048}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D8E07FD4-AA28-4079-AD13-1DC90844A900}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
+    </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2" uniqueCount="2">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3" uniqueCount="3">
   <si>
     <t>size</t>
   </si>
   <si>
-    <t>time</t>
+    <t>min</t>
+  </si>
+  <si>
+    <t>sec</t>
   </si>
 </sst>
 </file>
@@ -99,36 +108,6 @@
     </mc:Fallback>
   </mc:AlternateContent>
   <c:chart>
-    <c:title>
-      <c:overlay val="0"/>
-      <c:spPr>
-        <a:noFill/>
-        <a:ln>
-          <a:noFill/>
-        </a:ln>
-        <a:effectLst/>
-      </c:spPr>
-      <c:txPr>
-        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-        <a:lstStyle/>
-        <a:p>
-          <a:pPr>
-            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
-              <a:solidFill>
-                <a:schemeClr val="tx1">
-                  <a:lumMod val="65000"/>
-                  <a:lumOff val="35000"/>
-                </a:schemeClr>
-              </a:solidFill>
-              <a:latin typeface="+mn-lt"/>
-              <a:ea typeface="+mn-ea"/>
-              <a:cs typeface="+mn-cs"/>
-            </a:defRPr>
-          </a:pPr>
-          <a:endParaRPr lang="en-US"/>
-        </a:p>
-      </c:txPr>
-    </c:title>
     <c:autoTitleDeleted val="0"/>
     <c:plotArea>
       <c:layout/>
@@ -138,9 +117,6 @@
         <c:ser>
           <c:idx val="0"/>
           <c:order val="0"/>
-          <c:tx>
-            <c:v>time</c:v>
-          </c:tx>
           <c:spPr>
             <a:ln w="28575" cap="rnd">
               <a:solidFill>
@@ -155,10 +131,10 @@
           </c:marker>
           <c:cat>
             <c:numRef>
-              <c:f>Sheet1!$A$2:$A$8</c:f>
+              <c:f>Sheet1!$A$2:$A$13</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="7"/>
+                <c:ptCount val="12"/>
                 <c:pt idx="0">
                   <c:v>2</c:v>
                 </c:pt>
@@ -179,36 +155,66 @@
                 </c:pt>
                 <c:pt idx="6">
                   <c:v>8</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>9</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>10</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>11</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>12</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>13</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$B$2:$B$8</c:f>
+              <c:f>Sheet1!$C$2:$C$13</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="7"/>
+                <c:ptCount val="12"/>
                 <c:pt idx="0">
-                  <c:v>0.40414099999999997</c:v>
+                  <c:v>6.7356833333333333E-3</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0.41463450000000002</c:v>
+                  <c:v>6.9105750000000004E-3</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>21.056680799999999</c:v>
+                  <c:v>0.35094467999999995</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>16.589033700000002</c:v>
+                  <c:v>0.27648389500000004</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>2.5641554000000002</c:v>
+                  <c:v>4.2735923333333335E-2</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>8.4478250999999993</c:v>
+                  <c:v>0.14079708499999999</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>102.70711919999999</c:v>
+                  <c:v>1.7117853199999999</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>4.3178949999999992</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>25.350743333333334</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>34.092025</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>41.681003333333337</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>50.533431666666665</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -239,6 +245,61 @@
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="b"/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-GB"/>
+                  <a:t>Size of dungeon</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
@@ -304,6 +365,66 @@
             <a:effectLst/>
           </c:spPr>
         </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-GB"/>
+                  <a:t>Minutes</a:t>
+                </a:r>
+                <a:r>
+                  <a:rPr lang="en-GB" baseline="0"/>
+                  <a:t> to generate</a:t>
+                </a:r>
+                <a:endParaRPr lang="en-GB"/>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
@@ -1251,76 +1372,167 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:B8"/>
+  <dimension ref="A1:C13"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="N12" sqref="N12"/>
+      <selection activeCell="K25" sqref="K25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
       <c r="B1" t="s">
+        <v>2</v>
+      </c>
+      <c r="C1" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A2">
         <v>2</v>
       </c>
       <c r="B2">
         <v>0.40414099999999997</v>
       </c>
+      <c r="C2">
+        <f>B2/60</f>
+        <v>6.7356833333333333E-3</v>
+      </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A3">
         <v>3</v>
       </c>
       <c r="B3">
         <v>0.41463450000000002</v>
       </c>
+      <c r="C3">
+        <f t="shared" ref="C3:C13" si="0">B3/60</f>
+        <v>6.9105750000000004E-3</v>
+      </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A4">
         <v>4</v>
       </c>
       <c r="B4">
         <v>21.056680799999999</v>
       </c>
+      <c r="C4">
+        <f t="shared" si="0"/>
+        <v>0.35094467999999995</v>
+      </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A5">
         <v>5</v>
       </c>
       <c r="B5">
         <v>16.589033700000002</v>
       </c>
+      <c r="C5">
+        <f t="shared" si="0"/>
+        <v>0.27648389500000004</v>
+      </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A6">
         <v>6</v>
       </c>
       <c r="B6">
         <v>2.5641554000000002</v>
       </c>
+      <c r="C6">
+        <f t="shared" si="0"/>
+        <v>4.2735923333333335E-2</v>
+      </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A7">
         <v>7</v>
       </c>
       <c r="B7">
         <v>8.4478250999999993</v>
       </c>
+      <c r="C7">
+        <f t="shared" si="0"/>
+        <v>0.14079708499999999</v>
+      </c>
     </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A8">
         <v>8</v>
       </c>
       <c r="B8">
         <v>102.70711919999999</v>
+      </c>
+      <c r="C8">
+        <f t="shared" si="0"/>
+        <v>1.7117853199999999</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A9">
+        <v>9</v>
+      </c>
+      <c r="B9">
+        <v>259.07369999999997</v>
+      </c>
+      <c r="C9">
+        <f t="shared" si="0"/>
+        <v>4.3178949999999992</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A10">
+        <v>10</v>
+      </c>
+      <c r="B10">
+        <v>1521.0445999999999</v>
+      </c>
+      <c r="C10">
+        <f>B10/60</f>
+        <v>25.350743333333334</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A11">
+        <v>11</v>
+      </c>
+      <c r="B11">
+        <v>2045.5215000000001</v>
+      </c>
+      <c r="C11">
+        <f t="shared" si="0"/>
+        <v>34.092025</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A12">
+        <v>12</v>
+      </c>
+      <c r="B12">
+        <v>2500.8602000000001</v>
+      </c>
+      <c r="C12">
+        <f t="shared" si="0"/>
+        <v>41.681003333333337</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A13">
+        <v>13</v>
+      </c>
+      <c r="B13">
+        <v>3032.0059000000001</v>
+      </c>
+      <c r="C13">
+        <f t="shared" si="0"/>
+        <v>50.533431666666665</v>
       </c>
     </row>
   </sheetData>

</xml_diff>